<commit_message>
Se ha optimizado (y arreglado) la máquina de estados y sus estados. Se ha desacoplado todas las modificaciones de elementos GUI, a la lógica de la máquina de estados. Se ha creado una StatusBar, que de momento se usa para mostrar el estado actual de la máquina de estados a modo DEBUG. Pequeños (pero importantes) arreglos y mejoras a los elementos GUI.
</commit_message>
<xml_diff>
--- a/Plantillas.xlsx
+++ b/Plantillas.xlsx
@@ -358,10 +358,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R36"/>
+  <dimension ref="A1:R39"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:Q35"/>
+      <selection activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -386,11 +386,139 @@
     <col min="18" max="18" width="9.140625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="1" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="2:18" s="1" customFormat="1" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R5"/>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="L14" s="2"/>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="L15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="P15" s="2"/>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="L16" s="2"/>
+      <c r="N16" s="2"/>
+      <c r="P16" s="2"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="L17" s="2"/>
+      <c r="N17" s="2"/>
+      <c r="P17" s="2"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="L18" s="2"/>
+      <c r="N18" s="2"/>
+      <c r="P18" s="2"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="P19" s="1"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="P20" s="1"/>
+    </row>
+    <row r="21" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="P21" s="2"/>
+    </row>
+    <row r="22" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="D22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="J22" s="2"/>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="J23" s="2"/>
+    </row>
+    <row r="32" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L32" s="2"/>
+      <c r="P32" s="2"/>
+    </row>
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="J33" s="2"/>
+      <c r="L33" s="2"/>
+      <c r="N33" s="2"/>
+      <c r="P33" s="2"/>
+    </row>
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="J34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="N34" s="2"/>
+      <c r="P34" s="2"/>
+    </row>
+    <row r="35" spans="2:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="N35" s="2"/>
+      <c r="P35" s="2"/>
+    </row>
+    <row r="36" spans="2:16" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="P36" s="2"/>
+    </row>
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="L37" s="2"/>
+      <c r="N37" s="2"/>
+    </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="P39" s="1"/>
+    </row>
   </sheetData>
-  <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
+  <pageMargins left="0.45833333333333331" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se ha creado una clase en la que unir los datos obtenidos de los blobs mediante CV y la Figura asignada en función del tamaño. Para esta clase se ha implementado el método que dibuja, en el display principal, sobre las piezas, la figura asignada. Se ha creado una clase estática llamada Figures, que es una colección de objetos Figure configurados por el usuario, para establecer los rangos de áreas asignados a cada una.
</commit_message>
<xml_diff>
--- a/Plantillas.xlsx
+++ b/Plantillas.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tablero" sheetId="1" r:id="rId1"/>
+    <sheet name="Fichas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -24,7 +25,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -34,6 +35,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -50,10 +57,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,7 +368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R39"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
@@ -521,4 +529,227 @@
   <pageMargins left="0.45833333333333331" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3"/>
+      <c r="B1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+    </row>
+    <row r="2" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+    </row>
+    <row r="3" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+    </row>
+    <row r="5" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+    </row>
+    <row r="6" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+    </row>
+    <row r="7" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="8" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="2"/>
+    </row>
+    <row r="9" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="2"/>
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
+      <c r="Q9" s="2"/>
+    </row>
+    <row r="10" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
+      <c r="Q10" s="2"/>
+    </row>
+    <row r="11" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="K11" s="2"/>
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="2"/>
+    </row>
+    <row r="12" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:17" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" ht="32.1" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:7" ht="31.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+    </row>
+    <row r="20" spans="1:7" ht="31.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" ht="31.35" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:7" ht="31.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" ht="31.35" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.25" right="0.25" top="0.19791666666666666" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>